<commit_message>
Adicionado Timer de controle ao final do processo
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500ae9e30167d4d4/Documentos/PROJETOS/RPA/Gustavo MSG/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C4789056-C4EC-450B-9D4C-41FD8E1CC330}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B628488-D784-445F-A405-28BF43E90A52}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -646,7 +646,7 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -654,7 +654,7 @@
         <v>39</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -662,7 +662,7 @@
         <v>40</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -670,7 +670,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Correção do erro que permitia comentar mais de uma vez no mesmo usuario
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500ae9e30167d4d4/Documentos/PROJETOS/RPA/Gustavo MSG/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B628488-D784-445F-A405-28BF43E90A52}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{27E10D9A-C116-445D-A91E-C01F361B443A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -646,7 +646,7 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -654,7 +654,7 @@
         <v>39</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -662,7 +662,7 @@
         <v>40</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -670,7 +670,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>